<commit_message>
small change to the excel formula
</commit_message>
<xml_diff>
--- a/eTransfer-Form-Blank.xlsx
+++ b/eTransfer-Form-Blank.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\amy\eTranfers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czhu0\Documents\Reimburse\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9028AD71-32D0-4F37-9F96-27510009C84D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="2290" yWindow="2290" windowWidth="19200" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,18 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$36</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -89,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -471,49 +483,49 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +560,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -656,6 +674,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -691,6 +726,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -866,60 +918,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="31" x14ac:dyDescent="0.7">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.6">
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-    </row>
-    <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+    </row>
+    <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-    </row>
-    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+    </row>
+    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-    </row>
-    <row r="9" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+    </row>
+    <row r="9" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>1</v>
       </c>
@@ -930,159 +982,159 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
     </row>
-    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
       <c r="C12" s="21"/>
     </row>
-    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21"/>
     </row>
-    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
     </row>
-    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
     </row>
-    <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21"/>
     </row>
-    <row r="17" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
     </row>
-    <row r="18" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
     </row>
-    <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
     </row>
-    <row r="20" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
       <c r="B20" s="20"/>
       <c r="C20" s="21"/>
     </row>
-    <row r="21" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
     </row>
-    <row r="22" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="18"/>
       <c r="B22" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="17">
-        <f>SUM(C12:C21)</f>
+        <f>SUM(C11:C21)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-    </row>
-    <row r="25" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+    </row>
+    <row r="25" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-    </row>
-    <row r="26" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+    </row>
+    <row r="26" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="31" t="s">
         <v>17</v>
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="30"/>
     </row>
-    <row r="27" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-    </row>
-    <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+    </row>
+    <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
     </row>
-    <row r="29" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-    </row>
-    <row r="30" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+    </row>
+    <row r="30" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-    </row>
-    <row r="31" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+    </row>
+    <row r="31" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-    </row>
-    <row r="32" spans="1:3" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+    </row>
+    <row r="32" spans="1:3" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="6"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-    </row>
-    <row r="33" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+    </row>
+    <row r="33" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
-    </row>
-    <row r="34" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="41"/>
+      <c r="C33" s="42"/>
+    </row>
+    <row r="34" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
-    </row>
-    <row r="35" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="33"/>
+      <c r="C34" s="34"/>
+    </row>
+    <row r="35" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="34"/>
-    </row>
-    <row r="36" spans="1:3" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="35"/>
+      <c r="C35" s="36"/>
+    </row>
+    <row r="36" spans="1:3" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="25"/>
       <c r="B36" s="26"/>
       <c r="C36" s="27"/>
@@ -1109,24 +1161,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>